<commit_message>
Added drones in Agricutlure data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,19 +480,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.2765957446808511</v>
+        <v>0.277</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5232666356444858</v>
+        <v>0.523</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3053880832111238</v>
+        <v>0.305</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4376551203194129</v>
+        <v>0.438</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6398512749649903</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="3">
@@ -507,19 +507,75 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.723404255319149</v>
+        <v>0.723</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3161486996870616</v>
+        <v>0.316</v>
       </c>
       <c r="E3" t="n">
-        <v>0.575209817628723</v>
+        <v>0.575</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4885993485342019</v>
+        <v>0.489</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3028796868690006</v>
+        <v>0.303</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"geospatial data" OR "aerial photography" OR "irrigation management" OR "soil analysis" OR "smart farming" OR "yield estimation" OR "crop monitoring" OR "agricultural innovation" OR "drone technology" OR "climate monitoring" OR "weed detection" OR "pesticide spraying" OR "land surveying" OR "agricultural robotics" OR "aerial imaging" OR "variable rate application" OR "field surveillance" OR "agricultural drone" OR "drone mapping" OR "drones in agriculture" OR "harvest prediction" OR "crop scouting" OR "livestock tracking" OR "crop health assessment" OR "farm management software"
+</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.518</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.142</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"Drones in Agriculture"</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.592</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed mistake in results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -474,19 +474,18 @@
       <c r="B2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-"spinal stenosis" OR "spinal surgery risks" OR "cervical myelopathy" OR "gait disturbance" OR "corticosteroid injections" OR "degenerative disc disease" OR "surgery for myelopathy" OR "myelopathy symptoms" OR "nerve root compression" OR "upper limb weakness" OR "mri cervical spine" OR "cervical radiculopathy" OR "cervical spondylotic myelopathy" OR "myelopathy assessment" OR 
-(("rehabilitation" OR "long-term outcomes" OR "patient education" OR "pain management" OR "chronic pain" OR "physical therapy" OR "neurological symptoms" OR "postoperative care" OR "cervical spine" OR "neck pain" OR "reflex changes" OR "mobility issues" OR "spinal cord compression" OR "electromyography (emg)") AND ("Cervical Myelopathy"))
+"spinal stenosis" OR "spinal surgery risks" OR "cervical myelopathy" OR "gait disturbance" OR "corticosteroid injections" OR "degenerative disc disease" OR "surgery for myelopathy" OR "myelopathy symptoms" OR "nerve root compression" OR "upper limb weakness" OR "mri cervical spine" OR "cervical radiculopathy" OR "cervical spondylotic myelopathy" OR "myelopathy assessment"
 </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.277</v>
+        <v>0.723</v>
       </c>
       <c r="D2" t="n">
-        <v>0.523</v>
+        <v>0.316</v>
       </c>
       <c r="E2" t="n">
-        <v>0.305</v>
+        <v>0.575</v>
       </c>
       <c r="F2" t="n">
         <v>0.438</v>
@@ -507,13 +506,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.723</v>
+        <v>0.277</v>
       </c>
       <c r="D3" t="n">
-        <v>0.316</v>
+        <v>0.523</v>
       </c>
       <c r="E3" t="n">
-        <v>0.575</v>
+        <v>0.305</v>
       </c>
       <c r="F3" t="n">
         <v>0.489</v>

</xml_diff>

<commit_message>
Added prediction for - Robotic Arthroplasty - Soft Robotics - Crop Yield Prediction
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,6 +577,177 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"digital surgery" OR "surgical navigation" OR "haptic feedback" OR "robot-assisted surgery" OR "prosthetic devices" OR "computer-assisted surgery" OR "surgical workflow" OR (robotic arthroplasty) OR 
+(("clinical trials" OR "rehabilitation" OR "recovery time" OR "3d imaging" OR "patient satisfaction" OR "minimally invasive surgery" OR "surgical safety" OR "advanced imaging techniques" OR "orthopedic surgery" OR "total hip arthroplasty" OR "total knee arthroplasty" OR "biomechanics" OR "surgeon training" OR "motion planning" OR "joint replacement" OR "surgical precision" OR "robotic surgery" OR "implant technology" OR "surgery simulation" OR "surgical robotics") AND ("Arthoplasty"))
+</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.694</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Robotic Arthroplasty</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.401</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"compliant materials" OR (soft robotics) OR "soft actuators" OR "rehabilitation robotics" OR "pneumatic actuators" OR "robotic locomotion" OR "soft robotic systems" OR "soft robot control" OR "multi-material printing" OR "bio-inspired robotics" OR "continuum robots" OR "soft robot fabrication" OR "shape-morphing structures" OR "energy-efficient robotics" OR "soft robotic grippers" OR "soft exoskeletons" OR "soft robotic arms" OR "soft wearable robots" OR "autonomous soft robots" OR 
+(("material properties" OR "adaptive control" OR "sensor integration" OR "flexible materials" OR "human-robot interaction" OR "deformation mechanics" OR "lightweight structures" OR "soft sensors" OR "artificial muscles" OR "robotic manipulation") AND (Robot OR Soft))
+</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.487</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.644</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Soft Robotics</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.556</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.452</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.531</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.542</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"crop yield estimation" OR "crop simulation models" OR "yield forecasting" OR "soil health assessment" OR "precision agriculture" OR "sustainable farming practices" OR "weather pattern analysis" OR (crop yield prediction) OR "crop variety selection" OR "irrigation optimization" OR "technology adoption in agriculture" OR "agroecology" OR "data-driven agriculture" OR "economic viability of crops" OR 
+(("predictive modeling" OR "risk assessment" OR "climate change" OR "machine learning" OR "remote sensing" OR "land use change" OR "environmental impact assessment" OR "food security" OR "agricultural policies" OR "nutrient management" OR "satellite imagery" OR "farming systems analysis" OR "earth observation data" OR "phenotyping" OR "big data analytics" OR "climate resilience") AND ((Crop Yield)))
+</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Crop Yield Prediction</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.543</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.508</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.536</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added one SLR topic
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,6 +636,64 @@
         <v>0.536</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+("process adaptation" OR "processes adaptation" OR "customization of processes" OR "software processes customization" OR "software process customization" OR "customizing software processes" OR "process definition" OR "processes definition" OR "process composition" OR "compose processes" OR "processes composition" OR "process tailoring" OR "processes tailoring" OR "tailing of processes" OR "process development" OR "processes development" OR "process engineering" OR "processes engineering" OR "process design" OR "software process modelling" OR "software process modelling" OR "process implementation" OR "managing processes")
+AND
+("family of software process" OR "family of software processes" OR "families of software process" OR "families of software processes" OR "software process line" OR "software process lines" OR "software processes line" OR "software processes lines" OR "process-line" OR "process-lines" OR "processes-line" OR "processes-lines" OR "software process family" OR "software processes family" OR "software process families" OR "software processes families" OR "process-family" OR "processes-family" OR "process-families" OR "processes-families" OR "software process variability" OR "software process variabilities" OR "software processes variability" OR "software processes variabilities" OR "variabilities in software processes" OR "process domain engineering" OR "processes domain engineering" OR "process feature" OR "process features" OR "processes feature" OR "processes features" OR "process asset reuse")
+</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Software Process Line</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.575</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new topic: Resilience in Business and management
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -751,6 +751,63 @@
         <v>0.234</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"resilience assessment" OR "resilience strategies" OR "resilience evaluation" OR "resilience frameworks" OR "environmental resilience" OR "resilience as a capacity" OR "disaster recovery" OR "psychological resilience" OR "emotional resilience" OR "resourcefulness" OR "business continuity" OR "resilience training" OR "strategic flexibility" OR "continuity planning" OR "innovation resilience" OR "resilience culture" OR "resilience measurement" OR "organizational resilience" OR "operational resilience" OR "business agility" OR "team resilience" OR "resilience in leadership" OR "supply chain resilience" OR (resilience in business and management) OR 
+(("change management" OR "risk management" OR "sustainability" OR "adaptive capacity" OR "crisis management" OR "scenario planning" OR "stakeholder engagement" OR "crisis communication") AND (resilience and management))
+</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.222</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.499</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Resilience in Business and management</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.502</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New topic: Cervical Myelopathy
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -808,6 +808,62 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"spinal cord compression" OR "spinal stenosis" OR (cervical myelopathy) OR "gait disturbance" OR "degenerative disc disease" OR "spinal alignment" OR "myelopathy symptoms" OR "nerve root compression" OR "cervical spondylosis" OR "cervical spondylotic myelopathy" OR "upper motor neuron signs" OR 
+(("mri imaging" OR "cervical spine" OR "neurological examination" OR "emg studies" OR "reflex changes" OR "sensory loss" OR "decompression surgery") AND (Myelopathy))
+</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Cervical Myelopathy</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.787</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.636</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.752</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.699</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New topic: Drones in Agriculture
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -864,6 +864,63 @@
         <v>0.699</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"precision agriculture" OR "geospatial analysis" OR "aerial imagery" OR "pesticide spraying" OR "crop health assessment" OR "drone technology" OR "autonomous drones" OR "crop insurance" OR "agroecology" OR "farm management software" OR "agricultural robotics" OR "field scouting" OR (drones in agriculture) OR "agricultural drone" OR 
+(("yield estimation" OR "remote sensing" OR "variable rate application" OR "data analytics" OR "nutrient management" OR "land surveying" OR "unmanned aerial vehicle" OR "irrigation management" OR "climate monitoring" OR "sustainable farming" OR "farm productivity" OR "crop monitoring") AND (Drones OR Agriculture))
+</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.482</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.512</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Drones in Agriculture</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.049</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the rest of the topics
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -921,6 +921,461 @@
         <v>0.049</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"heritage tourism" OR "nature tourism" OR "tourist attractions" OR "hospitality industry" OR "economic impact of tourism" OR "rural tourism" OR "urban tourism" OR "ecotourism" OR "tourism infrastructure" OR "community-based tourism" OR "tourism investment" OR "medical tourism" OR "digital tourism" OR "tourism statistics" OR "responsible tourism" OR "seasonal tourism" OR "adventure tourism" OR (tourism growth nexus) OR 
+(("tourism development" OR "tourism management" OR "tourism marketing" OR "cultural tourism" OR "travel technology" OR "sustainable tourism" OR "destination management" OR "tourism policy" OR "business tourism" OR "global tourism" OR "travel trends" OR "tourist behavior") AND (Nexus))
+</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.095</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Tourism Growth Nexus</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.095</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"exergy analysis" OR "sustainable biofuel" OR "lifecycle assessment" OR "carbon neutrality" OR "algal biofuels" OR "food vs fuel debate" OR 
+(("waste-to-energy" OR "feedstock" OR "biodiesel" OR "economic viability" OR "bioenergy" OR "agricultural residues" OR "fossil fuel alternatives" OR "circular economy" OR "bioethanol" OR "energy independence") AND (Biofuel))
+</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.454</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.369</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sustainable Biofuel Economy</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"perovskite solar cells" OR "perovskite composition" OR "moisture resistance" OR "halide perovskites" OR "bandgap engineering" OR "photoelectric conversion" OR "mapbi3" OR "fapbi3" OR 
+(("efficiency" OR "stability" OR "degradation" OR "thermal stability" OR "nucleation" OR "doping effects" OR "fabrication techniques" OR "molecular dynamics simulations" OR "structural stability" OR "defect states" OR "scalability" OR "environmental stability" OR "lifespan" OR "energy conversion efficiency" OR "crystallization process" OR "interface stability" OR "photovoltaic performance" OR "solar energy conversion" OR "optoelectronic properties" OR "thin-film technology" OR "surface passivation" OR "charge carrier dynamics") AND (perovskite AND Solar))
+</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.461</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.8110000000000001</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Perovskite Solar Cells Stability</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.897</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.8149999999999999</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.481</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"nanocarriers" OR "nanoparticle characterization" OR "translational medicine" OR "camptothecin" OR "ribonucleotide reductase inhibitors" OR (nanopharmaceuticals) OR (nanonutraceuticals) OR 
+(("pharmacodynamics" OR "personalized medicine") AND (nanoparticles))
+</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.534</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.049</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Nanopharmaceuticals OR Nanonutraceuticals</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"climate action" OR "logistics efficiency" OR "circular economy" OR "sustainable logistics" OR "sustainable supply chain" OR "supply chain sustainability" OR "green building design" OR "inventory optimization" OR "green transportation" OR "eco-efficient processes" OR "carbon footprint reduction" OR "green certifications" OR "sustainable procurement" OR "warehouse automation" OR "eco-friendly packaging" OR "leed certification" OR "smart warehousing" OR "last mile delivery solutions" OR (green warehousing) OR "cold chain sustainability" OR 
+(("energy efficiency" OR "renewable energy" OR "emission reduction" OR "environmental impact assessment" OR "energy management systems" OR "waste management" OR "sustainable operations" OR "transport emissions" OR "green technologies" OR "resource optimization") AND (Warehousing))
+</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.432</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Green Warehousing</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.158</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.422</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.412</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"edge data processing" OR "distributed machine learning" OR "hardware acceleration" OR "deep learning inference" OR "edge infrastructure" OR "federated learning" OR "context-aware computing" OR "resource-constrained environments" OR "sensor data analytics" OR "smart edge applications" OR "edge-to-cloud architecture" OR "on-device ai" OR "latency-sensitive applications" OR "edge analytics" OR "ai model deployment" OR "edge ai devices" OR (ai on edge devices) OR "energy-efficient ai" OR "cognitive edge computing" OR "privacy-preserving ai" OR "ai inference engines" OR "scalability in edge ai" OR "ai multi-tenancy" OR 
+(("autonomous systems" OR "real-time data processing" OR "model compression" OR "internet of things (iot)" OR "low latency" OR "edge computing" OR "neural network optimization" OR "heterogeneous computing") AND (Edge Devices))
+</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.389</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AI on Edge Devices</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.483</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"smart healthcare" OR "mhealth" OR (internet of things in healthcare) OR "medical device integration" OR "internet of medical things" OR "smart hospitals" OR "ai in healthcare" OR "real-time health tracking" OR "healthcare interoperability" OR 
+(("chronic disease management" OR "health monitoring systems" OR "population health management" OR "wearable devices" OR "connected health" OR "digital health" OR "interoperability" OR "electronic health records" OR "patient engagement" OR "telemedicine" OR "virtual health" OR "personalized medicine" OR "remote patient monitoring" OR "health information exchange" OR "predictive analytics" OR "secure health data" OR "digital therapeutics" OR "health data analytics" OR "healthcare automation") AND (IoT))
+</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.517</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.676</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.543</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Internet of Things in Healthcare</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.326</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.341</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.377</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+"bioenergy" OR "decarbonization" OR (energy growth nexus)
+</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.046</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Energy Growth Nexus</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.045</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New evaluation Pipeline New results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,22 +446,42 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Semantic Precision</t>
+          <t>Cosine Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Semantic F2</t>
+          <t>Cosine F2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>MVVE Precision</t>
+          <t>Cluster Precision</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>MVVE F2</t>
+          <t>Cluster F2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MVEE Precision</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MVEE F2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Hull Precision</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Hull F2</t>
         </is>
       </c>
     </row>
@@ -473,23 +493,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>"digital surgery" OR "surgical navigation" OR "haptic feedback" OR "robot-assisted surgery" OR "prosthetic devices" OR "computer-assisted surgery" OR "surgical workflow" OR (robotic arthroplasty) OR (("clinical trials" OR "rehabilitation" OR "recovery time" OR "3d imaging" OR "patient satisfaction" OR "minimally invasive surgery" OR "surgical safety" OR "advanced imaging techniques" OR "orthopedic surgery" OR "total hip arthroplasty" OR "total knee arthroplasty" OR "biomechanics" OR "surgeon training" OR "motion planning" OR "joint replacement" OR "surgical precision" OR "robotic surgery" OR "implant technology" OR "surgery simulation" OR "surgical robotics") AND ("Arthoplasty"))</t>
+          <t>Robotic Arthroplasty</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>0.957</v>
       </c>
       <c r="D2" t="n">
-        <v>0.081</v>
+        <v>0.113</v>
       </c>
       <c r="E2" t="n">
-        <v>0.302</v>
+        <v>0.38</v>
       </c>
       <c r="F2" t="n">
-        <v>0.523</v>
+        <v>0.046</v>
       </c>
       <c r="G2" t="n">
-        <v>0.821</v>
+        <v>0.18</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="3">
@@ -500,23 +532,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Robotic Arthroplasty</t>
+          <t>"digital surgery" OR "surgical navigation" OR "haptic feedback" OR "robot-assisted surgery" OR "prosthetic devices" OR "computer-assisted surgery" OR "surgical workflow" OR (robotic arthroplasty) OR (("clinical trials" OR "rehabilitation" OR "recovery time" OR "3d imaging" OR "patient satisfaction" OR "minimally invasive surgery" OR "surgical safety" OR "advanced imaging techniques" OR "orthopedic surgery" OR "total hip arthroplasty" OR "total knee arthroplasty" OR "biomechanics" OR "surgeon training" OR "motion planning" OR "joint replacement" OR "surgical precision" OR "robotic surgery" OR "implant technology" OR "surgery simulation" OR "surgical robotics") AND ("Arthoplasty"))</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>0.957</v>
       </c>
       <c r="D3" t="n">
-        <v>0.72</v>
+        <v>0.858</v>
       </c>
       <c r="E3" t="n">
-        <v>0.898</v>
+        <v>0.93</v>
       </c>
       <c r="F3" t="n">
-        <v>0.483</v>
+        <v>0.574</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8</v>
+        <v>0.67</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.95</v>
       </c>
     </row>
     <row r="4">
@@ -527,23 +571,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>"compliant materials" OR (soft robotics) OR "soft actuators" OR "rehabilitation robotics" OR "pneumatic actuators" OR "robotic locomotion" OR "soft robotic systems" OR "soft robot control" OR "multi-material printing" OR "bio-inspired robotics" OR "continuum robots" OR "soft robot fabrication" OR "shape-morphing structures" OR "energy-efficient robotics" OR "soft robotic grippers" OR "soft exoskeletons" OR "soft robotic arms" OR "soft wearable robots" OR "autonomous soft robots" OR (("material properties" OR "adaptive control" OR "sensor integration" OR "flexible materials" OR "human-robot interaction" OR "deformation mechanics" OR "lightweight structures" OR "soft sensors" OR "artificial muscles" OR "robotic manipulation") AND (Robot OR Soft))</t>
+          <t>Soft Robotics</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.722</v>
+        <v>0.611</v>
       </c>
       <c r="D4" t="n">
-        <v>0.507</v>
+        <v>0.082</v>
       </c>
       <c r="E4" t="n">
-        <v>0.666</v>
+        <v>0.26</v>
       </c>
       <c r="F4" t="n">
-        <v>0.62</v>
+        <v>0.135</v>
       </c>
       <c r="G4" t="n">
-        <v>0.699</v>
+        <v>0.32</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.344</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.217</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.51</v>
       </c>
     </row>
     <row r="5">
@@ -554,23 +610,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Soft Robotics</t>
+          <t>"compliant materials" OR (soft robotics) OR "soft actuators" OR "rehabilitation robotics" OR "pneumatic actuators" OR "robotic locomotion" OR "soft robotic systems" OR "soft robot control" OR "multi-material printing" OR "bio-inspired robotics" OR "continuum robots" OR "soft robot fabrication" OR "shape-morphing structures" OR "energy-efficient robotics" OR "soft robotic grippers" OR "soft exoskeletons" OR "soft robotic arms" OR "soft wearable robots" OR "autonomous soft robots" OR (("material properties" OR "adaptive control" OR "sensor integration" OR "flexible materials" OR "human-robot interaction" OR "deformation mechanics" OR "lightweight structures" OR "soft sensors" OR "artificial muscles" OR "robotic manipulation") AND (Robot OR Soft))</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.556</v>
+        <v>0.528</v>
       </c>
       <c r="D5" t="n">
-        <v>0.755</v>
+        <v>0.195</v>
       </c>
       <c r="E5" t="n">
-        <v>0.587</v>
+        <v>0.39</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.282</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.37</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="6">
@@ -581,23 +649,35 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>"crop yield estimation" OR "crop simulation models" OR "yield forecasting" OR "soil health assessment" OR "precision agriculture" OR "sustainable farming practices" OR "weather pattern analysis" OR (crop yield prediction) OR "crop variety selection" OR "irrigation optimization" OR "technology adoption in agriculture" OR "agroecology" OR "data-driven agriculture" OR "economic viability of crops" OR (("predictive modeling" OR "risk assessment" OR "climate change" OR "machine learning" OR "remote sensing" OR "land use change" OR "environmental impact assessment" OR "food security" OR "agricultural policies" OR "nutrient management" OR "satellite imagery" OR "farming systems analysis" OR "earth observation data" OR "phenotyping" OR "big data analytics" OR "climate resilience") AND ((Crop Yield)))</t>
+          <t>Crop Yield Prediction</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.652</v>
+        <v>0.63</v>
       </c>
       <c r="D6" t="n">
-        <v>0.25</v>
+        <v>0.105</v>
       </c>
       <c r="E6" t="n">
-        <v>0.494</v>
+        <v>0.3</v>
       </c>
       <c r="F6" t="n">
-        <v>0.527</v>
+        <v>0.289</v>
       </c>
       <c r="G6" t="n">
-        <v>0.623</v>
+        <v>0.4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8159999999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.24</v>
       </c>
     </row>
     <row r="7">
@@ -608,23 +688,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Crop Yield Prediction</t>
+          <t>"crop yield estimation" OR "crop simulation models" OR "yield forecasting" OR "soil health assessment" OR "precision agriculture" OR "sustainable farming practices" OR "weather pattern analysis" OR (crop yield prediction) OR "crop variety selection" OR "irrigation optimization" OR "technology adoption in agriculture" OR "agroecology" OR "data-driven agriculture" OR "economic viability of crops" OR (("predictive modeling" OR "risk assessment" OR "climate change" OR "machine learning" OR "remote sensing" OR "land use change" OR "environmental impact assessment" OR "food security" OR "agricultural policies" OR "nutrient management" OR "satellite imagery" OR "farming systems analysis" OR "earth observation data" OR "phenotyping" OR "big data analytics" OR "climate resilience") AND ((Crop Yield)))</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.543</v>
+        <v>0.522</v>
       </c>
       <c r="D7" t="n">
-        <v>0.622</v>
+        <v>0.367</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="F7" t="n">
-        <v>0.551</v>
+        <v>0.407</v>
       </c>
       <c r="G7" t="n">
-        <v>0.545</v>
+        <v>0.47</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.861</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.88</v>
       </c>
     </row>
     <row r="8">
@@ -635,23 +727,35 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(synthetic biology) OR "genome editing" OR "microbial engineering" OR "synthetic organisms" OR "rna engineering" OR "environmental biotechnology" OR "bioprinting" OR "biomolecular engineering" OR "synthetic ecology" OR "synthetic genomics" OR "biomanufacturing" OR "biocontainment" OR "biodesign" OR "designer organisms" OR "chassis organisms" OR (("gene synthesis" OR "dna synthesis" OR "molecular biology" OR "systems biology" OR "bioinformatics" OR "cell-free systems" OR "protein engineering" OR "biotechnology" OR "directed evolution" OR "gene drives" OR "genetic engineering" OR "crispr" OR "synthetic pathways" OR "pathway engineering" OR "metabolic engineering") AND (Synthetic))</t>
+          <t>Synthetic Biology</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.586</v>
+        <v>0.517</v>
       </c>
       <c r="D8" t="n">
-        <v>0.552</v>
+        <v>0.056</v>
       </c>
       <c r="E8" t="n">
-        <v>0.579</v>
+        <v>0.19</v>
       </c>
       <c r="F8" t="n">
-        <v>0.532</v>
+        <v>0.172</v>
       </c>
       <c r="G8" t="n">
-        <v>0.574</v>
+        <v>0.34</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.501</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.49</v>
       </c>
     </row>
     <row r="9">
@@ -662,23 +766,35 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Synthetic Biology</t>
+          <t>(synthetic biology) OR "genome editing" OR "microbial engineering" OR "synthetic organisms" OR "rna engineering" OR "environmental biotechnology" OR "bioprinting" OR "biomolecular engineering" OR "synthetic ecology" OR "synthetic genomics" OR "biomanufacturing" OR "biocontainment" OR "biodesign" OR "designer organisms" OR "chassis organisms" OR (("gene synthesis" OR "dna synthesis" OR "molecular biology" OR "systems biology" OR "bioinformatics" OR "cell-free systems" OR "protein engineering" OR "biotechnology" OR "directed evolution" OR "gene drives" OR "genetic engineering" OR "crispr" OR "synthetic pathways" OR "pathway engineering" OR "metabolic engineering") AND (Synthetic))</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>0.207</v>
       </c>
       <c r="D9" t="n">
-        <v>0.619</v>
+        <v>0.098</v>
       </c>
       <c r="E9" t="n">
-        <v>0.239</v>
+        <v>0.17</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.357</v>
       </c>
       <c r="G9" t="n">
-        <v>0.237</v>
+        <v>0.2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.51</v>
       </c>
     </row>
     <row r="10">
@@ -689,23 +805,35 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>"resilience assessment" OR "resilience strategies" OR "resilience evaluation" OR "resilience frameworks" OR "environmental resilience" OR "resilience as a capacity" OR "disaster recovery" OR "psychological resilience" OR "emotional resilience" OR "resourcefulness" OR "business continuity" OR "resilience training" OR "strategic flexibility" OR "continuity planning" OR "innovation resilience" OR "resilience culture" OR "resilience measurement" OR "organizational resilience" OR "operational resilience" OR "business agility" OR "team resilience" OR "resilience in leadership" OR "supply chain resilience" OR (resilience in business and management) OR (("change management" OR "risk management" OR "sustainability" OR "adaptive capacity" OR "crisis management" OR "scenario planning" OR "stakeholder engagement" OR "crisis communication") AND (resilience and management))</t>
+          <t>Resilience in Business and management</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.222</v>
+        <v>0.148</v>
       </c>
       <c r="D10" t="n">
-        <v>0.29</v>
+        <v>0.011</v>
       </c>
       <c r="E10" t="n">
-        <v>0.233</v>
+        <v>0.04</v>
       </c>
       <c r="F10" t="n">
-        <v>0.419</v>
+        <v>0.162</v>
       </c>
       <c r="G10" t="n">
-        <v>0.245</v>
+        <v>0.19</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.27</v>
       </c>
     </row>
     <row r="11">
@@ -716,22 +844,34 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Resilience in Business and management</t>
+          <t>"resilience assessment" OR "resilience strategies" OR "resilience evaluation" OR "resilience frameworks" OR "environmental resilience" OR "resilience as a capacity" OR "disaster recovery" OR "psychological resilience" OR "emotional resilience" OR "resourcefulness" OR "business continuity" OR "resilience training" OR "strategic flexibility" OR "continuity planning" OR "innovation resilience" OR "resilience culture" OR "resilience measurement" OR "organizational resilience" OR "operational resilience" OR "business agility" OR "team resilience" OR "resilience in leadership" OR "supply chain resilience" OR (resilience in business and management) OR (("change management" OR "risk management" OR "sustainability" OR "adaptive capacity" OR "crisis management" OR "scenario planning" OR "stakeholder engagement" OR "crisis communication") AND (resilience and management))</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.484</v>
+        <v>0.028</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -743,23 +883,35 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>"spinal cord compression" OR "spinal stenosis" OR (cervical myelopathy) OR "gait disturbance" OR "degenerative disc disease" OR "spinal alignment" OR "myelopathy symptoms" OR "nerve root compression" OR "cervical spondylosis" OR "cervical spondylotic myelopathy" OR "upper motor neuron signs" OR (("mri imaging" OR "cervical spine" OR "neurological examination" OR "emg studies" OR "reflex changes" OR "sensory loss" OR "decompression surgery") AND (Myelopathy))</t>
+          <t>Cervical Myelopathy</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.872</v>
+        <v>0.851</v>
       </c>
       <c r="D12" t="n">
-        <v>0.454</v>
+        <v>0.252</v>
       </c>
       <c r="E12" t="n">
-        <v>0.737</v>
+        <v>0.51</v>
       </c>
       <c r="F12" t="n">
-        <v>0.488</v>
+        <v>0.105</v>
       </c>
       <c r="G12" t="n">
-        <v>0.754</v>
+        <v>0.31</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.53</v>
       </c>
     </row>
     <row r="13">
@@ -770,23 +922,35 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cervical Myelopathy</t>
+          <t>"spinal cord compression" OR "spinal stenosis" OR (cervical myelopathy) OR "gait disturbance" OR "degenerative disc disease" OR "spinal alignment" OR "myelopathy symptoms" OR "nerve root compression" OR "cervical spondylosis" OR "cervical spondylotic myelopathy" OR "upper motor neuron signs" OR (("mri imaging" OR "cervical spine" OR "neurological examination" OR "emg studies" OR "reflex changes" OR "sensory loss" OR "decompression surgery") AND (Myelopathy))</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.787</v>
+        <v>0.766</v>
       </c>
       <c r="D13" t="n">
-        <v>0.748</v>
+        <v>0.54</v>
       </c>
       <c r="E13" t="n">
-        <v>0.779</v>
+        <v>0.68</v>
       </c>
       <c r="F13" t="n">
-        <v>0.525</v>
+        <v>0.404</v>
       </c>
       <c r="G13" t="n">
-        <v>0.716</v>
+        <v>0.55</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.487</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="14">
@@ -797,23 +961,35 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>"precision agriculture" OR "geospatial analysis" OR "aerial imagery" OR "pesticide spraying" OR "crop health assessment" OR "drone technology" OR "autonomous drones" OR "crop insurance" OR "agroecology" OR "farm management software" OR "agricultural robotics" OR "field scouting" OR (drones in agriculture) OR "agricultural drone" OR (("yield estimation" OR "remote sensing" OR "variable rate application" OR "data analytics" OR "nutrient management" OR "land surveying" OR "unmanned aerial vehicle" OR "irrigation management" OR "climate monitoring" OR "sustainable farming" OR "farm productivity" OR "crop monitoring") AND (Drones OR Agriculture))</t>
+          <t>Drones in Agriculture</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="D14" t="n">
-        <v>0.271</v>
+        <v>0.074</v>
       </c>
       <c r="E14" t="n">
-        <v>0.439</v>
+        <v>0.22</v>
       </c>
       <c r="F14" t="n">
-        <v>0.492</v>
+        <v>0.309</v>
       </c>
       <c r="G14" t="n">
-        <v>0.514</v>
+        <v>0.33</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.38</v>
       </c>
     </row>
     <row r="15">
@@ -824,23 +1000,35 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Drones in Agriculture</t>
+          <t>"precision agriculture" OR "geospatial analysis" OR "aerial imagery" OR "pesticide spraying" OR "crop health assessment" OR "drone technology" OR "autonomous drones" OR "crop insurance" OR "agroecology" OR "farm management software" OR "agricultural robotics" OR "field scouting" OR (drones in agriculture) OR "agricultural drone" OR (("yield estimation" OR "remote sensing" OR "variable rate application" OR "data analytics" OR "nutrient management" OR "land surveying" OR "unmanned aerial vehicle" OR "irrigation management" OR "climate monitoring" OR "sustainable farming" OR "farm productivity" OR "crop monitoring") AND (Drones OR Agriculture))</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5679999999999999</v>
+        <v>0.232</v>
       </c>
       <c r="E15" t="n">
-        <v>0.049</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5</v>
+        <v>0.011</v>
       </c>
       <c r="G15" t="n">
-        <v>0.049</v>
+        <v>0.03</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -851,23 +1039,35 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>"heritage tourism" OR "nature tourism" OR "tourist attractions" OR "hospitality industry" OR "economic impact of tourism" OR "rural tourism" OR "urban tourism" OR "ecotourism" OR "tourism infrastructure" OR "community-based tourism" OR "tourism investment" OR "medical tourism" OR "digital tourism" OR "tourism statistics" OR "responsible tourism" OR "seasonal tourism" OR "adventure tourism" OR (tourism growth nexus) OR (("tourism development" OR "tourism management" OR "tourism marketing" OR "cultural tourism" OR "travel technology" OR "sustainable tourism" OR "destination management" OR "tourism policy" OR "business tourism" OR "global tourism" OR "travel trends" OR "tourist behavior") AND (Nexus))</t>
+          <t>Tourism Growth Nexus</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>0.08</v>
       </c>
       <c r="D16" t="n">
-        <v>0.005</v>
+        <v>0.008</v>
       </c>
       <c r="E16" t="n">
-        <v>0.019</v>
+        <v>0.03</v>
       </c>
       <c r="F16" t="n">
-        <v>0.484</v>
+        <v>0.569</v>
       </c>
       <c r="G16" t="n">
-        <v>0.096</v>
+        <v>0.05</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -878,23 +1078,35 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tourism Growth Nexus</t>
+          <t>"heritage tourism" OR "nature tourism" OR "tourist attractions" OR "hospitality industry" OR "economic impact of tourism" OR "rural tourism" OR "urban tourism" OR "ecotourism" OR "tourism infrastructure" OR "community-based tourism" OR "tourism investment" OR "medical tourism" OR "digital tourism" OR "tourism statistics" OR "responsible tourism" OR "seasonal tourism" OR "adventure tourism" OR (tourism growth nexus) OR (("tourism development" OR "tourism management" OR "tourism marketing" OR "cultural tourism" OR "travel technology" OR "sustainable tourism" OR "destination management" OR "tourism policy" OR "business tourism" OR "global tourism" OR "travel trends" OR "tourist behavior") AND (Nexus))</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>0.08</v>
       </c>
       <c r="D17" t="n">
-        <v>0.362</v>
+        <v>0.513</v>
       </c>
       <c r="E17" t="n">
-        <v>0.095</v>
+        <v>0.1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.465</v>
+        <v>0.259</v>
       </c>
       <c r="G17" t="n">
-        <v>0.096</v>
+        <v>0.09</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -905,23 +1117,35 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>"exergy analysis" OR "sustainable biofuel" OR "lifecycle assessment" OR "carbon neutrality" OR "algal biofuels" OR "food vs fuel debate" OR (("waste-to-energy" OR "feedstock" OR "biodiesel" OR "economic viability" OR "bioenergy" OR "agricultural residues" OR "fossil fuel alternatives" OR "circular economy" OR "bioethanol" OR "energy independence") AND (Biofuel))</t>
+          <t>Sustainable Biofuel Economy</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="D18" t="n">
-        <v>0.473</v>
+        <v>0.208</v>
       </c>
       <c r="E18" t="n">
-        <v>0.378</v>
+        <v>0.24</v>
       </c>
       <c r="F18" t="n">
-        <v>0.514</v>
+        <v>0.745</v>
       </c>
       <c r="G18" t="n">
-        <v>0.383</v>
+        <v>0.12</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.414</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.58</v>
       </c>
     </row>
     <row r="19">
@@ -932,23 +1156,35 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sustainable Biofuel Economy</t>
+          <t>"exergy analysis" OR "sustainable biofuel" OR "lifecycle assessment" OR "carbon neutrality" OR "algal biofuels" OR "food vs fuel debate" OR (("waste-to-energy" OR "feedstock" OR "biodiesel" OR "economic viability" OR "bioenergy" OR "agricultural residues" OR "fossil fuel alternatives" OR "circular economy" OR "bioethanol" OR "energy independence") AND (Biofuel))</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>0.02</v>
       </c>
       <c r="D19" t="n">
-        <v>0.619</v>
+        <v>0.314</v>
       </c>
       <c r="E19" t="n">
-        <v>0.025</v>
+        <v>0.02</v>
       </c>
       <c r="F19" t="n">
-        <v>0.499</v>
+        <v>0.012</v>
       </c>
       <c r="G19" t="n">
-        <v>0.025</v>
+        <v>0.02</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -959,23 +1195,35 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>"perovskite solar cells" OR "perovskite composition" OR "moisture resistance" OR "halide perovskites" OR "bandgap engineering" OR "photoelectric conversion" OR "mapbi3" OR "fapbi3" OR (("efficiency" OR "stability" OR "degradation" OR "thermal stability" OR "nucleation" OR "doping effects" OR "fabrication techniques" OR "molecular dynamics simulations" OR "structural stability" OR "defect states" OR "scalability" OR "environmental stability" OR "lifespan" OR "energy conversion efficiency" OR "crystallization process" OR "interface stability" OR "photovoltaic performance" OR "solar energy conversion" OR "optoelectronic properties" OR "thin-film technology" OR "surface passivation" OR "charge carrier dynamics") AND (perovskite AND Solar))</t>
+          <t>Perovskite Solar Cells Stability</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0.524</v>
+        <v>0.639</v>
       </c>
       <c r="E20" t="n">
-        <v>0.846</v>
+        <v>0.25</v>
       </c>
       <c r="F20" t="n">
-        <v>0.514</v>
+        <v>0.436</v>
       </c>
       <c r="G20" t="n">
-        <v>0.841</v>
+        <v>0.4</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="21">
@@ -986,23 +1234,35 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Perovskite Solar Cells Stability</t>
+          <t>"perovskite solar cells" OR "perovskite composition" OR "moisture resistance" OR "halide perovskites" OR "bandgap engineering" OR "photoelectric conversion" OR "mapbi3" OR "fapbi3" OR (("efficiency" OR "stability" OR "degradation" OR "thermal stability" OR "nucleation" OR "doping effects" OR "fabrication techniques" OR "molecular dynamics simulations" OR "structural stability" OR "defect states" OR "scalability" OR "environmental stability" OR "lifespan" OR "energy conversion efficiency" OR "crystallization process" OR "interface stability" OR "photovoltaic performance" OR "solar energy conversion" OR "optoelectronic properties" OR "thin-film technology" OR "surface passivation" OR "charge carrier dynamics") AND (perovskite AND Solar))</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>0.897</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.894</v>
       </c>
       <c r="E21" t="n">
-        <v>0.879</v>
+        <v>0.68</v>
       </c>
       <c r="F21" t="n">
-        <v>0.521</v>
+        <v>0.649</v>
       </c>
       <c r="G21" t="n">
-        <v>0.784</v>
+        <v>0.66</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.898</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.803</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.77</v>
       </c>
     </row>
     <row r="22">
@@ -1013,23 +1273,35 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>"nanocarriers" OR "nanoparticle characterization" OR "translational medicine" OR "camptothecin" OR "ribonucleotide reductase inhibitors" OR (nanopharmaceuticals) OR (nanonutraceuticals) OR (("pharmacodynamics" OR "personalized medicine") AND (nanoparticles))</t>
+          <t>Nanopharmaceuticals OR Nanonutraceuticals</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>0.04</v>
       </c>
       <c r="D22" t="n">
-        <v>0.888</v>
+        <v>0.197</v>
       </c>
       <c r="E22" t="n">
-        <v>0.049</v>
+        <v>0.04</v>
       </c>
       <c r="F22" t="n">
-        <v>0.517</v>
+        <v>0.624</v>
       </c>
       <c r="G22" t="n">
-        <v>0.049</v>
+        <v>0.01</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1040,22 +1312,34 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nanopharmaceuticals OR Nanonutraceuticals</t>
+          <t>"nanocarriers" OR "nanoparticle characterization" OR "translational medicine" OR "camptothecin" OR "ribonucleotide reductase inhibitors" OR (nanopharmaceuticals) OR (nanonutraceuticals) OR (("pharmacodynamics" OR "personalized medicine") AND (nanoparticles))</t>
         </is>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.996</v>
+        <v>0.19</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.425</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1067,23 +1351,35 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>"climate action" OR "logistics efficiency" OR "circular economy" OR "sustainable logistics" OR "sustainable supply chain" OR "supply chain sustainability" OR "green building design" OR "inventory optimization" OR "green transportation" OR "eco-efficient processes" OR "carbon footprint reduction" OR "green certifications" OR "sustainable procurement" OR "warehouse automation" OR "eco-friendly packaging" OR "leed certification" OR "smart warehousing" OR "last mile delivery solutions" OR (green warehousing) OR "cold chain sustainability" OR (("energy efficiency" OR "renewable energy" OR "emission reduction" OR "environmental impact assessment" OR "energy management systems" OR "waste management" OR "sustainable operations" OR "transport emissions" OR "green technologies" OR "resource optimization") AND (Warehousing))</t>
+          <t>Green Warehousing</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.237</v>
+        <v>0.158</v>
       </c>
       <c r="D24" t="n">
-        <v>0.281</v>
+        <v>0.002</v>
       </c>
       <c r="E24" t="n">
-        <v>0.245</v>
+        <v>0.01</v>
       </c>
       <c r="F24" t="n">
-        <v>0.529</v>
+        <v>0.108</v>
       </c>
       <c r="G24" t="n">
-        <v>0.266</v>
+        <v>0.16</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.352</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.54</v>
       </c>
     </row>
     <row r="25">
@@ -1094,23 +1390,35 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Green Warehousing</t>
+          <t>"climate action" OR "logistics efficiency" OR "circular economy" OR "sustainable logistics" OR "sustainable supply chain" OR "supply chain sustainability" OR "green building design" OR "inventory optimization" OR "green transportation" OR "eco-efficient processes" OR "carbon footprint reduction" OR "green certifications" OR "sustainable procurement" OR "warehouse automation" OR "eco-friendly packaging" OR "leed certification" OR "smart warehousing" OR "last mile delivery solutions" OR (green warehousing) OR "cold chain sustainability" OR (("energy efficiency" OR "renewable energy" OR "emission reduction" OR "environmental impact assessment" OR "energy management systems" OR "waste management" OR "sustainable operations" OR "transport emissions" OR "green technologies" OR "resource optimization") AND (Warehousing))</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.158</v>
+        <v>0.105</v>
       </c>
       <c r="D25" t="n">
-        <v>0.797</v>
+        <v>0.203</v>
       </c>
       <c r="E25" t="n">
-        <v>0.188</v>
+        <v>0.12</v>
       </c>
       <c r="F25" t="n">
-        <v>0.604</v>
+        <v>0.519</v>
       </c>
       <c r="G25" t="n">
-        <v>0.185</v>
+        <v>0.18</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.44</v>
       </c>
     </row>
     <row r="26">
@@ -1121,23 +1429,35 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>"edge data processing" OR "distributed machine learning" OR "hardware acceleration" OR "deep learning inference" OR "edge infrastructure" OR "federated learning" OR "context-aware computing" OR "resource-constrained environments" OR "sensor data analytics" OR "smart edge applications" OR "edge-to-cloud architecture" OR "on-device ai" OR "latency-sensitive applications" OR "edge analytics" OR "ai model deployment" OR "edge ai devices" OR (ai on edge devices) OR "energy-efficient ai" OR "cognitive edge computing" OR "privacy-preserving ai" OR "ai inference engines" OR "scalability in edge ai" OR "ai multi-tenancy" OR (("autonomous systems" OR "real-time data processing" OR "model compression" OR "internet of things (iot)" OR "low latency" OR "edge computing" OR "neural network optimization" OR "heterogeneous computing") AND (Edge Devices))</t>
+          <t>AI on Edge Devices</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.389</v>
+        <v>0.333</v>
       </c>
       <c r="D26" t="n">
-        <v>0.636</v>
+        <v>0.11</v>
       </c>
       <c r="E26" t="n">
-        <v>0.422</v>
+        <v>0.23</v>
       </c>
       <c r="F26" t="n">
-        <v>0.493</v>
+        <v>0.586</v>
       </c>
       <c r="G26" t="n">
-        <v>0.406</v>
+        <v>0.12</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.44</v>
       </c>
     </row>
     <row r="27">
@@ -1148,23 +1468,35 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>AI on Edge Devices</t>
+          <t>"edge data processing" OR "distributed machine learning" OR "hardware acceleration" OR "deep learning inference" OR "edge infrastructure" OR "federated learning" OR "context-aware computing" OR "resource-constrained environments" OR "sensor data analytics" OR "smart edge applications" OR "edge-to-cloud architecture" OR "on-device ai" OR "latency-sensitive applications" OR "edge analytics" OR "ai model deployment" OR "edge ai devices" OR (ai on edge devices) OR "energy-efficient ai" OR "cognitive edge computing" OR "privacy-preserving ai" OR "ai inference engines" OR "scalability in edge ai" OR "ai multi-tenancy" OR (("autonomous systems" OR "real-time data processing" OR "model compression" OR "internet of things (iot)" OR "low latency" OR "edge computing" OR "neural network optimization" OR "heterogeneous computing") AND (Edge Devices))</t>
         </is>
       </c>
       <c r="C27" t="n">
         <v>0.111</v>
       </c>
       <c r="D27" t="n">
-        <v>0.868</v>
+        <v>0.315</v>
       </c>
       <c r="E27" t="n">
-        <v>0.135</v>
+        <v>0.13</v>
       </c>
       <c r="F27" t="n">
-        <v>0.516</v>
+        <v>0.536</v>
       </c>
       <c r="G27" t="n">
-        <v>0.132</v>
+        <v>0.1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.11</v>
       </c>
     </row>
     <row r="28">
@@ -1175,23 +1507,35 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>"smart healthcare" OR "mhealth" OR (internet of things in healthcare) OR "medical device integration" OR "internet of medical things" OR "smart hospitals" OR "ai in healthcare" OR "real-time health tracking" OR "healthcare interoperability" OR (("chronic disease management" OR "health monitoring systems" OR "population health management" OR "wearable devices" OR "connected health" OR "digital health" OR "interoperability" OR "electronic health records" OR "patient engagement" OR "telemedicine" OR "virtual health" OR "personalized medicine" OR "remote patient monitoring" OR "health information exchange" OR "predictive analytics" OR "secure health data" OR "digital therapeutics" OR "health data analytics" OR "healthcare automation") AND (IoT))</t>
+          <t>Internet of Things in Healthcare</t>
         </is>
       </c>
       <c r="C28" t="n">
         <v>0.517</v>
       </c>
       <c r="D28" t="n">
-        <v>0.404</v>
+        <v>0.177</v>
       </c>
       <c r="E28" t="n">
-        <v>0.49</v>
+        <v>0.35</v>
       </c>
       <c r="F28" t="n">
-        <v>0.471</v>
+        <v>0.448</v>
       </c>
       <c r="G28" t="n">
-        <v>0.507</v>
+        <v>0.29</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.53</v>
       </c>
     </row>
     <row r="29">
@@ -1202,23 +1546,35 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Internet of Things in Healthcare</t>
+          <t>"smart healthcare" OR "mhealth" OR (internet of things in healthcare) OR "medical device integration" OR "internet of medical things" OR "smart hospitals" OR "ai in healthcare" OR "real-time health tracking" OR "healthcare interoperability" OR (("chronic disease management" OR "health monitoring systems" OR "population health management" OR "wearable devices" OR "connected health" OR "digital health" OR "interoperability" OR "electronic health records" OR "patient engagement" OR "telemedicine" OR "virtual health" OR "personalized medicine" OR "remote patient monitoring" OR "health information exchange" OR "predictive analytics" OR "secure health data" OR "digital therapeutics" OR "health data analytics" OR "healthcare automation") AND (IoT))</t>
         </is>
       </c>
       <c r="C29" t="n">
         <v>0.345</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.365</v>
       </c>
       <c r="E29" t="n">
-        <v>0.383</v>
+        <v>0.34</v>
       </c>
       <c r="F29" t="n">
-        <v>0.458</v>
+        <v>0.538</v>
       </c>
       <c r="G29" t="n">
-        <v>0.363</v>
+        <v>0.28</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.79</v>
       </c>
     </row>
     <row r="30">
@@ -1229,23 +1585,35 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>"bioenergy" OR "decarbonization" OR (energy growth nexus)</t>
+          <t>Energy Growth Nexus</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.032</v>
+        <v>0.021</v>
       </c>
       <c r="E30" t="n">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.555</v>
+        <v>0.016</v>
       </c>
       <c r="G30" t="n">
-        <v>0.046</v>
+        <v>0.03</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1256,23 +1624,35 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Energy Growth Nexus</t>
+          <t>"bioenergy" OR "decarbonization" OR (energy growth nexus)</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.037</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.42</v>
+        <v>0.287</v>
       </c>
       <c r="E31" t="n">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.613</v>
+        <v>0.01</v>
       </c>
       <c r="G31" t="n">
-        <v>0.046</v>
+        <v>0.02</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1283,23 +1663,35 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>("process adaptation" OR "processes adaptation" OR "customization of processes" OR "software processes customization" OR "software process customization" OR "customizing software processes" OR "process definition" OR "processes definition" OR "process composition" OR "compose processes" OR "processes composition" OR "process tailoring" OR "processes tailoring" OR "tailing of processes" OR "process development" OR "processes development" OR "process engineering" OR "processes engineering" OR "process design" OR "software process modelling" OR "software process modelling" OR "process implementation" OR "managing processes") AND ("family of software process" OR "family of software processes" OR "families of software process" OR "families of software processes" OR "software process line" OR "software process lines" OR "software processes line" OR "software processes lines" OR "process-line" OR "process-lines" OR "processes-line" OR "processes-lines" OR "software process family" OR "software processes family" OR "software process families" OR "software processes families" OR "process-family" OR "processes-family" OR "process-families" OR "processes-families" OR "software process variability" OR "software process variabilities" OR "software processes variability" OR "software processes variabilities" OR "variabilities in software processes" OR "process domain engineering" OR "processes domain engineering" OR "process feature" OR "process features" OR "processes feature" OR "processes features" OR "process asset reuse")</t>
+          <t>Software Process Line</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.372</v>
+        <v>0.349</v>
       </c>
       <c r="D32" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.287</v>
       </c>
       <c r="E32" t="n">
-        <v>0.41</v>
+        <v>0.33</v>
       </c>
       <c r="F32" t="n">
-        <v>0.386</v>
+        <v>0.396</v>
       </c>
       <c r="G32" t="n">
-        <v>0.375</v>
+        <v>0.38</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.277</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="33">
@@ -1310,23 +1702,35 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Software Process Line</t>
+          <t>("process adaptation" OR "processes adaptation" OR "customization of processes" OR "software processes customization" OR "software process customization" OR "customizing software processes" OR "process definition" OR "processes definition" OR "process composition" OR "compose processes" OR "processes composition" OR "process tailoring" OR "processes tailoring" OR "tailing of processes" OR "process development" OR "processes development" OR "process engineering" OR "processes engineering" OR "process design" OR "software process modelling" OR "software process modelling" OR "process implementation" OR "managing processes") AND ("family of software process" OR "family of software processes" OR "families of software process" OR "families of software processes" OR "software process line" OR "software process lines" OR "software processes line" OR "software processes lines" OR "process-line" OR "process-lines" OR "processes-line" OR "processes-lines" OR "software process family" OR "software processes family" OR "software process families" OR "software processes families" OR "process-family" OR "processes-family" OR "process-families" OR "processes-families" OR "software process variability" OR "software process variabilities" OR "software processes variability" OR "software processes variabilities" OR "variabilities in software processes" OR "process domain engineering" OR "processes domain engineering" OR "process feature" OR "process features" OR "processes feature" OR "processes features" OR "process asset reuse")</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.605</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>0.369</v>
+        <v>0.017</v>
       </c>
       <c r="E33" t="n">
-        <v>0.536</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F33" t="n">
-        <v>0.429</v>
+        <v>0.077</v>
       </c>
       <c r="G33" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.24</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.28</v>
       </c>
     </row>
     <row r="34">
@@ -1337,23 +1741,35 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>(stream processing OR "continuous query" OR "stream-based system" OR "data stream system" OR "streaming system" OR "complex event processing") AND ("adapt" OR "reconfigur" ) AND ("latency" OR "response time")</t>
+          <t>Data Stream Processing Latency</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.13</v>
+        <v>0.101</v>
       </c>
       <c r="D34" t="n">
-        <v>0.642</v>
+        <v>0.242</v>
       </c>
       <c r="E34" t="n">
-        <v>0.155</v>
+        <v>0.11</v>
       </c>
       <c r="F34" t="n">
-        <v>0.481</v>
+        <v>0.173</v>
       </c>
       <c r="G34" t="n">
-        <v>0.153</v>
+        <v>0.11</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.177</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.52</v>
       </c>
     </row>
     <row r="35">
@@ -1364,23 +1780,35 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Data Stream Processing Latency</t>
+          <t>(stream processing OR "continuous query" OR "stream-based system" OR "data stream system" OR "streaming system" OR "complex event processing") AND ("adapt" OR "reconfigur" ) AND ("latency" OR "response time")</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.188</v>
+        <v>0.174</v>
       </c>
       <c r="D35" t="n">
-        <v>0.635</v>
+        <v>0.263</v>
       </c>
       <c r="E35" t="n">
-        <v>0.219</v>
+        <v>0.19</v>
       </c>
       <c r="F35" t="n">
-        <v>0.46</v>
+        <v>0.494</v>
       </c>
       <c r="G35" t="n">
-        <v>0.214</v>
+        <v>0.21</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="36">
@@ -1391,23 +1819,35 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>("metamodel" OR "meta-model") AND ("business process" OR "process model" OR "petrinet" OR "petri-net" OR "workflow" OR "Declare")</t>
+          <t>Business Process Meta Models</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.654</v>
+        <v>0.577</v>
       </c>
       <c r="D36" t="n">
-        <v>0.585</v>
+        <v>0.254</v>
       </c>
       <c r="E36" t="n">
-        <v>0.639</v>
+        <v>0.46</v>
       </c>
       <c r="F36" t="n">
-        <v>0.521</v>
+        <v>0.258</v>
       </c>
       <c r="G36" t="n">
-        <v>0.622</v>
+        <v>0.4</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.5649999999999999</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.77</v>
       </c>
     </row>
     <row r="37">
@@ -1418,23 +1858,35 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Business Process Meta Models</t>
+          <t>("metamodel" OR "meta-model") AND ("business process" OR "process model" OR "petrinet" OR "petri-net" OR "workflow" OR "Declare")</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>0.308</v>
       </c>
       <c r="D37" t="n">
-        <v>0.494</v>
+        <v>0.222</v>
       </c>
       <c r="E37" t="n">
-        <v>0.333</v>
+        <v>0.29</v>
       </c>
       <c r="F37" t="n">
-        <v>0.525</v>
+        <v>0.34</v>
       </c>
       <c r="G37" t="n">
-        <v>0.335</v>
+        <v>0.31</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.22</v>
       </c>
     </row>
     <row r="38">
@@ -1445,22 +1897,34 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (("Parallel Programming") AND Modeling) OR (Multicore AND (Modeling OR "Software Engineering")) OR (Multicore AND ("Parallel Programming")) AND ("Modeling" OR "Software Engineering")</t>
+          <t>Multicore Performance Prediction</t>
         </is>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.889</v>
+        <v>0.519</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.444</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1472,22 +1936,34 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Multicore Performance Prediction</t>
+          <t xml:space="preserve"> (("Parallel Programming") AND Modeling) OR (Multicore AND (Modeling OR "Software Engineering")) OR (Multicore AND ("Parallel Programming")) AND ("Modeling" OR "Software Engineering")</t>
         </is>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.872</v>
+        <v>0.299</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.518</v>
+        <v>1</v>
       </c>
       <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1499,22 +1975,34 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>((migration OR evolution OR adaptation OR transformation OR modernization OR reengineering OR integration OR adoption OR switching) AND (monolithic OR legacy OR existing OR preexisting OR on-premise) AND (system OR software OR application) AND (cloud AND (software OR application OR architecture OR infrastructure OR cloud environment)))</t>
+          <t>Cloud Migration</t>
         </is>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.531</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1526,22 +2014,34 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Cloud Migration</t>
+          <t>((migration OR evolution OR adaptation OR transformation OR modernization OR reengineering OR integration OR adoption OR switching) AND (monolithic OR legacy OR existing OR preexisting OR on-premise) AND (system OR software OR application) AND (cloud AND (software OR application OR architecture OR infrastructure OR cloud environment)))</t>
         </is>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1553,23 +2053,35 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>software AND (metric OR measurement) AND (fault OR defect* OR quality OR error-prone) AND (predict* OR prone* OR probability OR assess* OR detect* OR estimat* OR classificat*)</t>
+          <t>Software Fault Prediction Metrics</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.792</v>
       </c>
       <c r="D42" t="n">
-        <v>0.134</v>
+        <v>0.074</v>
       </c>
       <c r="E42" t="n">
-        <v>0.403</v>
+        <v>0.27</v>
       </c>
       <c r="F42" t="n">
-        <v>0.45</v>
+        <v>0.39</v>
       </c>
       <c r="G42" t="n">
-        <v>0.7</v>
+        <v>0.63</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.42</v>
       </c>
     </row>
     <row r="43">
@@ -1580,23 +2092,35 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Software Fault Prediction Metrics</t>
+          <t>software AND (metric OR measurement) AND (fault OR defect* OR quality OR error-prone) AND (predict* OR prone* OR probability OR assess* OR detect* OR estimat* OR classificat*)</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>0.25</v>
       </c>
       <c r="D43" t="n">
-        <v>0.806</v>
+        <v>0.617</v>
       </c>
       <c r="E43" t="n">
-        <v>0.29</v>
+        <v>0.28</v>
       </c>
       <c r="F43" t="n">
-        <v>0.434</v>
+        <v>0.329</v>
       </c>
       <c r="G43" t="n">
-        <v>0.273</v>
+        <v>0.21</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.49</v>
       </c>
     </row>
     <row r="44">
@@ -1607,23 +2131,35 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>(software OR applicati* OR systems ) AND (fault* OR defect* OR quality OR error-prone) AND (predict*OR prone* OR probability OR assess* OR detect* OR estimat* OR classificat*)</t>
+          <t>Software Defect Prediction</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.2</v>
+        <v>0.204</v>
       </c>
       <c r="D44" t="n">
-        <v>0.443</v>
+        <v>0.022</v>
       </c>
       <c r="E44" t="n">
-        <v>0.225</v>
+        <v>0.08</v>
       </c>
       <c r="F44" t="n">
-        <v>0.625</v>
+        <v>0.02</v>
       </c>
       <c r="G44" t="n">
-        <v>0.231</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.06</v>
       </c>
     </row>
     <row r="45">
@@ -1634,23 +2170,35 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Software Defect Prediction</t>
+          <t>(software OR applicati* OR systems ) AND (fault* OR defect* OR quality OR error-prone) AND (predict*OR prone* OR probability OR assess* OR detect* OR estimat* OR classificat*)</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.327</v>
+        <v>0.315</v>
       </c>
       <c r="D45" t="n">
-        <v>0.945</v>
+        <v>0.574</v>
       </c>
       <c r="E45" t="n">
-        <v>0.376</v>
+        <v>0.34</v>
       </c>
       <c r="F45" t="n">
-        <v>0.555</v>
+        <v>0.466</v>
       </c>
       <c r="G45" t="n">
-        <v>0.357</v>
+        <v>0.28</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.628</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the decayed_f2 to decayed_precision
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -512,16 +512,16 @@
         <v>0.18</v>
       </c>
       <c r="H2" t="n">
-        <v>0.155</v>
+        <v>0.13</v>
       </c>
       <c r="I2" t="n">
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="J2" t="n">
-        <v>0.119</v>
+        <v>0.114</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="3">
@@ -551,16 +551,16 @@
         <v>0.67</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9</v>
+        <v>0.871</v>
       </c>
       <c r="I3" t="n">
         <v>0.97</v>
       </c>
       <c r="J3" t="n">
-        <v>0.786</v>
+        <v>0.771</v>
       </c>
       <c r="K3" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -590,16 +590,16 @@
         <v>0.32</v>
       </c>
       <c r="H4" t="n">
-        <v>0.344</v>
+        <v>0.302</v>
       </c>
       <c r="I4" t="n">
-        <v>0.51</v>
+        <v>0.6</v>
       </c>
       <c r="J4" t="n">
-        <v>0.217</v>
+        <v>0.222</v>
       </c>
       <c r="K4" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="5">
@@ -626,19 +626,19 @@
         <v>0.282</v>
       </c>
       <c r="G5" t="n">
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
       <c r="H5" t="n">
-        <v>0.423</v>
+        <v>0.529</v>
       </c>
       <c r="I5" t="n">
-        <v>0.73</v>
+        <v>0.82</v>
       </c>
       <c r="J5" t="n">
-        <v>0.303</v>
+        <v>0.317</v>
       </c>
       <c r="K5" t="n">
-        <v>0.66</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -659,25 +659,25 @@
         <v>0.105</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="F6" t="n">
         <v>0.289</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4</v>
+        <v>0.47</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8159999999999999</v>
+        <v>0.532</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06</v>
+        <v>0.58</v>
       </c>
       <c r="J6" t="n">
-        <v>0.618</v>
+        <v>0.3</v>
       </c>
       <c r="K6" t="n">
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7">
@@ -698,25 +698,25 @@
         <v>0.367</v>
       </c>
       <c r="E7" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="F7" t="n">
         <v>0.407</v>
       </c>
       <c r="G7" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="H7" t="n">
-        <v>0.861</v>
+        <v>0.783</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="J7" t="n">
-        <v>0.724</v>
+        <v>0.516</v>
       </c>
       <c r="K7" t="n">
-        <v>0.88</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="8">
@@ -737,25 +737,25 @@
         <v>0.056</v>
       </c>
       <c r="E8" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F8" t="n">
         <v>0.172</v>
       </c>
       <c r="G8" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="H8" t="n">
-        <v>0.501</v>
+        <v>0.454</v>
       </c>
       <c r="I8" t="n">
-        <v>0.39</v>
+        <v>0.62</v>
       </c>
       <c r="J8" t="n">
-        <v>0.391</v>
+        <v>0.388</v>
       </c>
       <c r="K8" t="n">
-        <v>0.49</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="9">
@@ -782,19 +782,19 @@
         <v>0.357</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="H9" t="n">
-        <v>0.325</v>
+        <v>0.154</v>
       </c>
       <c r="I9" t="n">
-        <v>0.63</v>
+        <v>0.47</v>
       </c>
       <c r="J9" t="n">
-        <v>0.182</v>
+        <v>0.094</v>
       </c>
       <c r="K9" t="n">
-        <v>0.51</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="10">
@@ -821,19 +821,19 @@
         <v>0.162</v>
       </c>
       <c r="G10" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="H10" t="n">
-        <v>0.14</v>
+        <v>0.133</v>
       </c>
       <c r="I10" t="n">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="J10" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="K10" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="11">
@@ -893,7 +893,7 @@
         <v>0.252</v>
       </c>
       <c r="E12" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="F12" t="n">
         <v>0.105</v>
@@ -902,16 +902,16 @@
         <v>0.31</v>
       </c>
       <c r="H12" t="n">
-        <v>0.47</v>
+        <v>0.542</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5</v>
+        <v>0.66</v>
       </c>
       <c r="J12" t="n">
-        <v>0.423</v>
+        <v>0.466</v>
       </c>
       <c r="K12" t="n">
-        <v>0.53</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="13">
@@ -932,7 +932,7 @@
         <v>0.54</v>
       </c>
       <c r="E13" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="F13" t="n">
         <v>0.404</v>
@@ -941,16 +941,16 @@
         <v>0.55</v>
       </c>
       <c r="H13" t="n">
-        <v>0.57</v>
+        <v>0.626</v>
       </c>
       <c r="I13" t="n">
-        <v>0.83</v>
+        <v>0.88</v>
       </c>
       <c r="J13" t="n">
-        <v>0.487</v>
+        <v>0.492</v>
       </c>
       <c r="K13" t="n">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="14">
@@ -977,19 +977,19 @@
         <v>0.309</v>
       </c>
       <c r="G14" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="H14" t="n">
-        <v>0.183</v>
+        <v>0.256</v>
       </c>
       <c r="I14" t="n">
-        <v>0.48</v>
+        <v>0.58</v>
       </c>
       <c r="J14" t="n">
-        <v>0.114</v>
+        <v>0.154</v>
       </c>
       <c r="K14" t="n">
-        <v>0.38</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="15">
@@ -1055,7 +1055,7 @@
         <v>0.569</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05</v>
+        <v>0.09</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1127,25 +1127,25 @@
         <v>0.208</v>
       </c>
       <c r="E18" t="n">
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
       <c r="F18" t="n">
         <v>0.745</v>
       </c>
       <c r="G18" t="n">
-        <v>0.12</v>
+        <v>0.32</v>
       </c>
       <c r="H18" t="n">
-        <v>0.625</v>
+        <v>0.73</v>
       </c>
       <c r="I18" t="n">
-        <v>0.43</v>
+        <v>0.63</v>
       </c>
       <c r="J18" t="n">
-        <v>0.414</v>
+        <v>0.512</v>
       </c>
       <c r="K18" t="n">
-        <v>0.58</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="19">
@@ -1205,25 +1205,25 @@
         <v>0.639</v>
       </c>
       <c r="E20" t="n">
-        <v>0.25</v>
+        <v>0.52</v>
       </c>
       <c r="F20" t="n">
         <v>0.436</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H20" t="n">
-        <v>0.755</v>
+        <v>0.637</v>
       </c>
       <c r="I20" t="n">
-        <v>0.13</v>
+        <v>0.52</v>
       </c>
       <c r="J20" t="n">
-        <v>0.638</v>
+        <v>0.508</v>
       </c>
       <c r="K20" t="n">
-        <v>0.25</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="21">
@@ -1244,25 +1244,25 @@
         <v>0.894</v>
       </c>
       <c r="E21" t="n">
-        <v>0.68</v>
+        <v>0.84</v>
       </c>
       <c r="F21" t="n">
         <v>0.649</v>
       </c>
       <c r="G21" t="n">
-        <v>0.66</v>
+        <v>0.73</v>
       </c>
       <c r="H21" t="n">
-        <v>0.898</v>
+        <v>0.641</v>
       </c>
       <c r="I21" t="n">
-        <v>0.75</v>
+        <v>0.86</v>
       </c>
       <c r="J21" t="n">
-        <v>0.803</v>
+        <v>0.58</v>
       </c>
       <c r="K21" t="n">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="22">
@@ -1283,13 +1283,13 @@
         <v>0.197</v>
       </c>
       <c r="E22" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F22" t="n">
         <v>0.624</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1370,16 +1370,16 @@
         <v>0.16</v>
       </c>
       <c r="H24" t="n">
-        <v>0.352</v>
+        <v>0.337</v>
       </c>
       <c r="I24" t="n">
-        <v>0.53</v>
+        <v>0.63</v>
       </c>
       <c r="J24" t="n">
-        <v>0.275</v>
+        <v>0.167</v>
       </c>
       <c r="K24" t="n">
-        <v>0.54</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="25">
@@ -1409,16 +1409,16 @@
         <v>0.18</v>
       </c>
       <c r="H25" t="n">
-        <v>0.182</v>
+        <v>0.112</v>
       </c>
       <c r="I25" t="n">
-        <v>0.53</v>
+        <v>0.39</v>
       </c>
       <c r="J25" t="n">
-        <v>0.134</v>
+        <v>0.08</v>
       </c>
       <c r="K25" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26">
@@ -1445,19 +1445,19 @@
         <v>0.586</v>
       </c>
       <c r="G26" t="n">
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="H26" t="n">
-        <v>0.318</v>
+        <v>0.331</v>
       </c>
       <c r="I26" t="n">
-        <v>0.51</v>
+        <v>0.61</v>
       </c>
       <c r="J26" t="n">
-        <v>0.149</v>
+        <v>0.182</v>
       </c>
       <c r="K26" t="n">
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27">
@@ -1487,16 +1487,16 @@
         <v>0.1</v>
       </c>
       <c r="H27" t="n">
-        <v>0.059</v>
+        <v>0.082</v>
       </c>
       <c r="I27" t="n">
-        <v>0.24</v>
+        <v>0.31</v>
       </c>
       <c r="J27" t="n">
-        <v>0.025</v>
+        <v>0.034</v>
       </c>
       <c r="K27" t="n">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="28">
@@ -1517,25 +1517,25 @@
         <v>0.177</v>
       </c>
       <c r="E28" t="n">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="F28" t="n">
         <v>0.448</v>
       </c>
       <c r="G28" t="n">
-        <v>0.29</v>
+        <v>0.42</v>
       </c>
       <c r="H28" t="n">
-        <v>0.47</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I28" t="n">
-        <v>0.48</v>
+        <v>0.38</v>
       </c>
       <c r="J28" t="n">
-        <v>0.393</v>
+        <v>0.498</v>
       </c>
       <c r="K28" t="n">
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="29">
@@ -1556,25 +1556,25 @@
         <v>0.365</v>
       </c>
       <c r="E29" t="n">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="F29" t="n">
         <v>0.538</v>
       </c>
       <c r="G29" t="n">
-        <v>0.28</v>
+        <v>0.3</v>
       </c>
       <c r="H29" t="n">
-        <v>0.659</v>
+        <v>0.852</v>
       </c>
       <c r="I29" t="n">
-        <v>0.8</v>
+        <v>0.92</v>
       </c>
       <c r="J29" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.649</v>
       </c>
       <c r="K29" t="n">
-        <v>0.79</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="30">
@@ -1682,16 +1682,16 @@
         <v>0.38</v>
       </c>
       <c r="H32" t="n">
-        <v>0.267</v>
+        <v>0.248</v>
       </c>
       <c r="I32" t="n">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="J32" t="n">
-        <v>0.277</v>
+        <v>0.257</v>
       </c>
       <c r="K32" t="n">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="33">
@@ -1721,16 +1721,16 @@
         <v>0.24</v>
       </c>
       <c r="H33" t="n">
-        <v>0.098</v>
+        <v>0.129</v>
       </c>
       <c r="I33" t="n">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="J33" t="n">
-        <v>0.073</v>
+        <v>0.095</v>
       </c>
       <c r="K33" t="n">
-        <v>0.28</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="34">
@@ -1760,16 +1760,16 @@
         <v>0.11</v>
       </c>
       <c r="H34" t="n">
-        <v>0.238</v>
+        <v>0.242</v>
       </c>
       <c r="I34" t="n">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="J34" t="n">
-        <v>0.177</v>
+        <v>0.212</v>
       </c>
       <c r="K34" t="n">
-        <v>0.52</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="35">
@@ -1799,16 +1799,16 @@
         <v>0.21</v>
       </c>
       <c r="H35" t="n">
-        <v>0.408</v>
+        <v>0.378</v>
       </c>
       <c r="I35" t="n">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="J35" t="n">
-        <v>0.316</v>
+        <v>0.257</v>
       </c>
       <c r="K35" t="n">
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="36">
@@ -1838,16 +1838,16 @@
         <v>0.4</v>
       </c>
       <c r="H36" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.594</v>
       </c>
       <c r="I36" t="n">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="J36" t="n">
-        <v>0.404</v>
+        <v>0.393</v>
       </c>
       <c r="K36" t="n">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="37">
@@ -1877,16 +1877,16 @@
         <v>0.31</v>
       </c>
       <c r="H37" t="n">
-        <v>0.09</v>
+        <v>0.095</v>
       </c>
       <c r="I37" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="J37" t="n">
-        <v>0.054</v>
+        <v>0.059</v>
       </c>
       <c r="K37" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="38">
@@ -2069,19 +2069,19 @@
         <v>0.39</v>
       </c>
       <c r="G42" t="n">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="H42" t="n">
-        <v>0.18</v>
+        <v>0.167</v>
       </c>
       <c r="I42" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="J42" t="n">
-        <v>0.126</v>
+        <v>0.115</v>
       </c>
       <c r="K42" t="n">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="43">
@@ -2111,13 +2111,13 @@
         <v>0.21</v>
       </c>
       <c r="H43" t="n">
-        <v>0.238</v>
+        <v>0.308</v>
       </c>
       <c r="I43" t="n">
-        <v>0.61</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="J43" t="n">
-        <v>0.161</v>
+        <v>0.163</v>
       </c>
       <c r="K43" t="n">
         <v>0.49</v>
@@ -2150,16 +2150,16 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="H44" t="n">
-        <v>0.029</v>
+        <v>0.022</v>
       </c>
       <c r="I44" t="n">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="J44" t="n">
-        <v>0.014</v>
+        <v>0.011</v>
       </c>
       <c r="K44" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="45">
@@ -2180,7 +2180,7 @@
         <v>0.574</v>
       </c>
       <c r="E45" t="n">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="F45" t="n">
         <v>0.466</v>
@@ -2189,16 +2189,16 @@
         <v>0.28</v>
       </c>
       <c r="H45" t="n">
-        <v>0.628</v>
+        <v>0.586</v>
       </c>
       <c r="I45" t="n">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="J45" t="n">
-        <v>0.497</v>
+        <v>0.445</v>
       </c>
       <c r="K45" t="n">
-        <v>0.83</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced SLR query results with SQW results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -512,16 +512,16 @@
         <v>0.18</v>
       </c>
       <c r="H2" t="n">
-        <v>0.135</v>
+        <v>0.128</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="J2" t="n">
-        <v>0.112</v>
+        <v>0.122</v>
       </c>
       <c r="K2" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="3">
@@ -551,16 +551,16 @@
         <v>0.67</v>
       </c>
       <c r="H3" t="n">
-        <v>0.838</v>
+        <v>0.835</v>
       </c>
       <c r="I3" t="n">
         <v>0.95</v>
       </c>
       <c r="J3" t="n">
-        <v>0.752</v>
+        <v>0.801</v>
       </c>
       <c r="K3" t="n">
-        <v>0.92</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -590,13 +590,13 @@
         <v>0.26</v>
       </c>
       <c r="H4" t="n">
-        <v>0.313</v>
+        <v>0.362</v>
       </c>
       <c r="I4" t="n">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="J4" t="n">
-        <v>0.226</v>
+        <v>0.216</v>
       </c>
       <c r="K4" t="n">
         <v>0.3</v>
@@ -629,13 +629,13 @@
         <v>0.35</v>
       </c>
       <c r="H5" t="n">
-        <v>0.61</v>
+        <v>0.654</v>
       </c>
       <c r="I5" t="n">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J5" t="n">
-        <v>0.423</v>
+        <v>0.368</v>
       </c>
       <c r="K5" t="n">
         <v>0.6</v>
@@ -668,16 +668,16 @@
         <v>0.22</v>
       </c>
       <c r="H6" t="n">
-        <v>0.398</v>
+        <v>0.477</v>
       </c>
       <c r="I6" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="J6" t="n">
-        <v>0.305</v>
+        <v>0.295</v>
       </c>
       <c r="K6" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="7">
@@ -707,16 +707,16 @@
         <v>0.45</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.738</v>
       </c>
       <c r="I7" t="n">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="J7" t="n">
-        <v>0.57</v>
+        <v>0.529</v>
       </c>
       <c r="K7" t="n">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="8">
@@ -746,16 +746,16 @@
         <v>0.26</v>
       </c>
       <c r="H8" t="n">
-        <v>0.741</v>
+        <v>0.822</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0.382</v>
+        <v>0.62</v>
       </c>
       <c r="K8" t="n">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9">
@@ -785,16 +785,16 @@
         <v>0.18</v>
       </c>
       <c r="H9" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.185</v>
       </c>
       <c r="I9" t="n">
-        <v>0.29</v>
+        <v>0.42</v>
       </c>
       <c r="J9" t="n">
-        <v>0.047</v>
+        <v>0.11</v>
       </c>
       <c r="K9" t="n">
-        <v>0.19</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="10">
@@ -824,16 +824,16 @@
         <v>0.17</v>
       </c>
       <c r="H10" t="n">
-        <v>0.103</v>
+        <v>0.15</v>
       </c>
       <c r="I10" t="n">
-        <v>0.29</v>
+        <v>0.33</v>
       </c>
       <c r="J10" t="n">
-        <v>0.046</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="K10" t="n">
-        <v>0.18</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="11">
@@ -902,16 +902,16 @@
         <v>0.27</v>
       </c>
       <c r="H12" t="n">
-        <v>0.577</v>
+        <v>0.573</v>
       </c>
       <c r="I12" t="n">
         <v>0.05</v>
       </c>
       <c r="J12" t="n">
-        <v>0.505</v>
+        <v>0.476</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="13">
@@ -941,16 +941,16 @@
         <v>0.52</v>
       </c>
       <c r="H13" t="n">
-        <v>0.663</v>
+        <v>0.634</v>
       </c>
       <c r="I13" t="n">
         <v>0.75</v>
       </c>
       <c r="J13" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.493</v>
       </c>
       <c r="K13" t="n">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="14">
@@ -980,16 +980,16 @@
         <v>0.19</v>
       </c>
       <c r="H14" t="n">
-        <v>0.133</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="I14" t="n">
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
       <c r="J14" t="n">
-        <v>0.061</v>
+        <v>0.028</v>
       </c>
       <c r="K14" t="n">
-        <v>0.22</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15">
@@ -1136,16 +1136,16 @@
         <v>0.02</v>
       </c>
       <c r="H18" t="n">
-        <v>0.636</v>
+        <v>0.513</v>
       </c>
       <c r="I18" t="n">
-        <v>0.06</v>
+        <v>0.15</v>
       </c>
       <c r="J18" t="n">
-        <v>0.402</v>
+        <v>0.343</v>
       </c>
       <c r="K18" t="n">
-        <v>0.26</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="19">
@@ -1214,13 +1214,13 @@
         <v>0.1</v>
       </c>
       <c r="H20" t="n">
-        <v>0.979</v>
+        <v>0.977</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0.954</v>
+        <v>0.88</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1253,16 +1253,16 @@
         <v>0.53</v>
       </c>
       <c r="H21" t="n">
-        <v>0.984</v>
+        <v>0.926</v>
       </c>
       <c r="I21" t="n">
-        <v>0.43</v>
+        <v>0.47</v>
       </c>
       <c r="J21" t="n">
-        <v>0.912</v>
+        <v>0.798</v>
       </c>
       <c r="K21" t="n">
-        <v>0.48</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="22">
@@ -1370,13 +1370,13 @@
         <v>0.15</v>
       </c>
       <c r="H24" t="n">
-        <v>0.299</v>
+        <v>0.365</v>
       </c>
       <c r="I24" t="n">
-        <v>0.26</v>
+        <v>0.19</v>
       </c>
       <c r="J24" t="n">
-        <v>0.155</v>
+        <v>0.186</v>
       </c>
       <c r="K24" t="n">
         <v>0.33</v>
@@ -1409,16 +1409,16 @@
         <v>0.18</v>
       </c>
       <c r="H25" t="n">
-        <v>0.198</v>
+        <v>0.342</v>
       </c>
       <c r="I25" t="n">
-        <v>0.55</v>
+        <v>0.72</v>
       </c>
       <c r="J25" t="n">
-        <v>0.118</v>
+        <v>0.182</v>
       </c>
       <c r="K25" t="n">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="26">
@@ -1448,13 +1448,13 @@
         <v>0.01</v>
       </c>
       <c r="H26" t="n">
-        <v>0.301</v>
+        <v>0.264</v>
       </c>
       <c r="I26" t="n">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="J26" t="n">
-        <v>0.141</v>
+        <v>0.162</v>
       </c>
       <c r="K26" t="n">
         <v>0.31</v>
@@ -1487,16 +1487,16 @@
         <v>0.1</v>
       </c>
       <c r="H27" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.082</v>
       </c>
       <c r="I27" t="n">
-        <v>0.27</v>
+        <v>0.31</v>
       </c>
       <c r="J27" t="n">
-        <v>0.032</v>
+        <v>0.024</v>
       </c>
       <c r="K27" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="28">
@@ -1526,16 +1526,16 @@
         <v>0.12</v>
       </c>
       <c r="H28" t="n">
-        <v>0.436</v>
+        <v>0.434</v>
       </c>
       <c r="I28" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="J28" t="n">
-        <v>0.354</v>
+        <v>0.332</v>
       </c>
       <c r="K28" t="n">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="29">
@@ -1565,13 +1565,13 @@
         <v>0.28</v>
       </c>
       <c r="H29" t="n">
-        <v>0.587</v>
+        <v>0.58</v>
       </c>
       <c r="I29" t="n">
         <v>0.65</v>
       </c>
       <c r="J29" t="n">
-        <v>0.48</v>
+        <v>0.441</v>
       </c>
       <c r="K29" t="n">
         <v>0.65</v>
@@ -1589,31 +1589,31 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.349</v>
+        <v>0.605</v>
       </c>
       <c r="D30" t="n">
-        <v>0.307</v>
+        <v>0.02</v>
       </c>
       <c r="E30" t="n">
-        <v>0.34</v>
+        <v>0.09</v>
       </c>
       <c r="F30" t="n">
-        <v>0.396</v>
+        <v>0.316</v>
       </c>
       <c r="G30" t="n">
-        <v>0.38</v>
+        <v>0.22</v>
       </c>
       <c r="H30" t="n">
-        <v>0.287</v>
+        <v>0.701</v>
       </c>
       <c r="I30" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0.287</v>
+        <v>0.261</v>
       </c>
       <c r="K30" t="n">
-        <v>0.67</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>("process adaptation" OR "processes adaptation" OR "customization of processes" OR "software processes customization" OR "software process customization" OR "customizing software processes" OR "process definition" OR "processes definition" OR "process composition" OR "compose processes" OR "processes composition" OR "process tailoring" OR "processes tailoring" OR "tailing of processes" OR "process development" OR "processes development" OR "process engineering" OR "processes engineering" OR "process design" OR "software process modelling" OR "software process modelling" OR "process implementation" OR "managing processes") AND ("family of software process" OR "family of software processes" OR "families of software process" OR "families of software processes" OR "software process line" OR "software process lines" OR "software processes line" OR "software processes lines" OR "process-line" OR "process-lines" OR "processes-line" OR "processes-lines" OR "software process family" OR "software processes family" OR "software process families" OR "software processes families" OR "process-family" OR "processes-family" OR "process-families" OR "processes-families" OR "software process variability" OR "software process variabilities" OR "software processes variability" OR "software processes variabilities" OR "variabilities in software processes" OR "process domain engineering" OR "processes domain engineering" OR "process feature" OR "process features" OR "processes feature" OR "processes features" OR "process asset reuse")</t>
+          <t>"software development methodologies" OR "software project management" OR (software process line) OR "code review processes" OR "risk management in software" OR "software testing strategies" OR "software documentation" OR "agile software development" OR "process maturity model" OR "software quality assurance" OR "user acceptance testing" OR "agile methodologies" OR "software development lifecycle" OR "software product line engineering" OR "software engineering best practices" OR "devops practices" OR (("process modeling" OR "system design" OR "change management" OR "process optimization" OR "process automation" OR "maintenance processes" OR "performance metrics" OR "iterative development" OR "software architecture" OR "continuous integration" OR "requirements engineering" OR "software process improvement" OR "release management" OR "configuration management" OR "version control systems" OR "stakeholder engagement") AND (Software Process))</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1643,16 +1643,16 @@
         <v>0.24</v>
       </c>
       <c r="H31" t="n">
-        <v>0.102</v>
+        <v>0.749</v>
       </c>
       <c r="I31" t="n">
-        <v>0.35</v>
+        <v>0.66</v>
       </c>
       <c r="J31" t="n">
-        <v>0.065</v>
+        <v>0.298</v>
       </c>
       <c r="K31" t="n">
-        <v>0.25</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32">
@@ -1667,31 +1667,31 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.101</v>
+        <v>0.261</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3</v>
+        <v>0.016</v>
       </c>
       <c r="E32" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="F32" t="n">
-        <v>0.173</v>
+        <v>0.014</v>
       </c>
       <c r="G32" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="K32" t="n">
         <v>0.11</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.269</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0.215</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0.58</v>
       </c>
     </row>
     <row r="33">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>(stream processing OR "continuous query" OR "stream-based system" OR "data stream system" OR "streaming system" OR "complex event processing") AND ("adapt" OR "reconfigur" ) AND ("latency" OR "response time")</t>
+          <t>"field-programmable gate arrays" OR "low-latency processing" OR "real-time analytics" OR "concept drift" OR "stream benchmarks" OR "workload variations" OR "reactive programming" OR "memory reuse" OR "floating-point units" OR "edge stream processing" OR "query latency" OR (data stream processing latency) OR "dataflow programming" OR "push-based streaming" OR "microbenchmarks" OR "rpc mechanisms" OR "dma management" OR "pull-based streaming" OR "scoreboarding" OR "ingestion/storage integration" OR (("sensor data" OR "distributed data processing" OR "parallel processing" OR "stream processing" OR "scalability" OR "adaptability" OR "kernel functions" OR "edge computing" OR "shared memory" OR "streaming algorithms" OR "bandwidth optimization" OR "compiler tools" OR "hardware acceleration" OR "graphics processing units" OR "pipelining") AND (Processing Latency))</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1721,16 +1721,16 @@
         <v>0.21</v>
       </c>
       <c r="H33" t="n">
-        <v>0.401</v>
+        <v>0.271</v>
       </c>
       <c r="I33" t="n">
-        <v>0.76</v>
+        <v>0.65</v>
       </c>
       <c r="J33" t="n">
-        <v>0.298</v>
+        <v>0.222</v>
       </c>
       <c r="K33" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="34">
@@ -1745,31 +1745,31 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.577</v>
+        <v>0.615</v>
       </c>
       <c r="D34" t="n">
-        <v>0.299</v>
+        <v>0.061</v>
       </c>
       <c r="E34" t="n">
-        <v>0.49</v>
+        <v>0.21</v>
       </c>
       <c r="F34" t="n">
-        <v>0.258</v>
+        <v>0.107</v>
       </c>
       <c r="G34" t="n">
-        <v>0.4</v>
+        <v>0.26</v>
       </c>
       <c r="H34" t="n">
-        <v>0.471</v>
+        <v>0.152</v>
       </c>
       <c r="I34" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.39</v>
       </c>
       <c r="J34" t="n">
-        <v>0.4</v>
+        <v>0.112</v>
       </c>
       <c r="K34" t="n">
-        <v>0.77</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="35">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>("metamodel" OR "meta-model") AND ("business process" OR "process model" OR "petrinet" OR "petri-net" OR "workflow" OR "Declare")</t>
+          <t>"business rules" OR "business process frameworks" OR "workflow management" OR "enterprise architecture" OR "lean management" OR "requirements gathering" OR "six sigma" OR "business process reengineering" OR "bpmn" OR "organizational process assets" OR (business process meta models) OR (("process analysis" OR "process improvement" OR "process simulation" OR "change management" OR "risk management" OR "knowledge management" OR "process optimization" OR "continuous improvement" OR "modeling languages" OR "process automation" OR "process mapping" OR "performance metrics" OR "business process management" OR "quality assurance" OR "stakeholder analysis" OR "business process modeling" OR "value chain analysis" OR "process governance" OR "process documentation") AND (business metamodels))</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1799,16 +1799,16 @@
         <v>0.31</v>
       </c>
       <c r="H35" t="n">
-        <v>0.323</v>
+        <v>0.38</v>
       </c>
       <c r="I35" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="J35" t="n">
-        <v>0.228</v>
+        <v>0.26</v>
       </c>
       <c r="K35" t="n">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="36">
@@ -1823,31 +1823,31 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.273</v>
       </c>
       <c r="D36" t="n">
-        <v>0.574</v>
+        <v>0.118</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>0.158</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="37">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (("Parallel Programming") AND Modeling) OR (Multicore AND (Modeling OR "Software Engineering")) OR (Multicore AND ("Parallel Programming")) AND ("Modeling" OR "Software Engineering")</t>
+          <t>"data locality" OR "system bottlenecks" OR "computational throughput" OR "memory bandwidth" OR "workload distribution" OR "core utilization" OR "simd" OR "interconnect bandwidth" OR "thread management" OR "multicore processors" OR "hardware threading" OR "multicore architecture" OR "task granularity" OR "resource contention" OR "cache coherence" OR "reuse profiles" OR (multicore performance prediction) OR "amdahl's law" OR (("performance modeling" OR "energy efficiency" OR "analytical modeling" OR "performance prediction" OR "latency" OR "performance metrics" OR "scheduling algorithms" OR "scalability" OR "load balancing" OR "parallel computing" OR "software optimization" OR "benchmarking" OR "task scheduling") AND (Multicore Performance))</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>((migration OR evolution OR adaptation OR transformation OR modernization OR reengineering OR integration OR adoption OR switching) AND (monolithic OR legacy OR existing OR preexisting OR on-premise) AND (system OR software OR application) AND (cloud AND (software OR application OR architecture OR infrastructure OR cloud environment)))</t>
+          <t>"virtualization" OR "cloud strategy" OR "cloud optimization" OR "disaster recovery" OR "hybrid cloud" OR "cloud scalability" OR "cloud transformation" OR (cloud migration) OR "cloud adoption" OR "cloud cost optimization" OR "cloud compliance" OR "cloud backup" OR "cloud native applications" OR "serverless computing" OR "devops in cloud" OR "iaas migration" OR "paas migration" OR "saas migration" OR (("data migration" OR "application migration" OR "cloud services" OR "cloud networking" OR "cloud performance" OR "cloud management" OR "cloud security" OR "cloud architecture" OR "multi-cloud" OR "cloud storage" OR "cloud monitoring" OR "cloud infrastructure") AND (Cloud Migration))</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1979,31 +1979,31 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="D40" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.078</v>
       </c>
       <c r="E40" t="n">
-        <v>0.29</v>
+        <v>0.24</v>
       </c>
       <c r="F40" t="n">
-        <v>0.39</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>0.54</v>
+        <v>0.23</v>
       </c>
       <c r="H40" t="n">
-        <v>0.176</v>
+        <v>0.254</v>
       </c>
       <c r="I40" t="n">
-        <v>0.47</v>
+        <v>0.53</v>
       </c>
       <c r="J40" t="n">
-        <v>0.119</v>
+        <v>0.15</v>
       </c>
       <c r="K40" t="n">
-        <v>0.38</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="41">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>software AND (metric OR measurement) AND (fault OR defect* OR quality OR error-prone) AND (predict* OR prone* OR probability OR assess* OR detect* OR estimat* OR classificat*)</t>
+          <t>"defect identification" OR "software quality" OR "software complexity" OR "change-proneness" OR "metric validation" OR "cost evaluation framework" OR "fault prediction models" OR "testing resource allocation" OR "fault-proneness" OR "source code metrics" OR "software maintainability" OR "software metrics suite" OR "internal software metrics" OR (software fault prediction metrics) OR "fault-prone classes" OR "apache ecosystem" OR "eclipse ecosystem" OR "sonarqube rules" OR (("predictive models" OR "performance evaluation" OR "statistical methods" OR "data quality" OR "reliability" OR "empirical study" OR "comments" OR "statistical correlation" OR "machine learning" OR "classification techniques" OR "prediction accuracy" OR "inheritance" OR "open-source systems" OR "ensemble methods" OR "cohesion" OR "ensemble learning" OR "generalizability") AND (software error prediction))</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -2033,16 +2033,16 @@
         <v>0.21</v>
       </c>
       <c r="H41" t="n">
-        <v>0.194</v>
+        <v>0.248</v>
       </c>
       <c r="I41" t="n">
-        <v>0.55</v>
+        <v>0.62</v>
       </c>
       <c r="J41" t="n">
-        <v>0.155</v>
+        <v>0.138</v>
       </c>
       <c r="K41" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="42">
@@ -2057,31 +2057,31 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.204</v>
+        <v>0.519</v>
       </c>
       <c r="D42" t="n">
-        <v>0.024</v>
+        <v>0.142</v>
       </c>
       <c r="E42" t="n">
-        <v>0.08</v>
+        <v>0.32</v>
       </c>
       <c r="F42" t="n">
-        <v>0.02</v>
+        <v>0.155</v>
       </c>
       <c r="G42" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="H42" t="n">
-        <v>0.023</v>
+        <v>0.603</v>
       </c>
       <c r="I42" t="n">
-        <v>0.11</v>
+        <v>0.51</v>
       </c>
       <c r="J42" t="n">
-        <v>0.013</v>
+        <v>0.402</v>
       </c>
       <c r="K42" t="n">
-        <v>0.06</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="43">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>(software OR applicati* OR systems ) AND (fault* OR defect* OR quality OR error-prone) AND (predict*OR prone* OR probability OR assess* OR detect* OR estimat* OR classificat*)</t>
+          <t>"software maintenance" OR "software metrics" OR "model transparency" OR "ensemble classification" OR "defect localization" OR "effort metrics" OR "software artifacts" OR "defect prediction models" OR "quality assurance resources" OR "heterogeneous classifiers" OR (software defect prediction) OR "software sizing metrics" OR "model explainability" OR "post-release defects" OR "static code metrics" OR "historical defect information" OR "cyclomatic complexity" OR "defect-prone modules" OR "source code similarity metrics" OR "cross-company project metrics" OR (("predictive models" OR "cost model" OR "testing costs" OR "machine learning" OR "defectiveness" OR "software quality" OR "resource allocation" OR "defect density" OR "quality assurance" OR "defect repair" OR "project-level information") AND (Software defect))</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -2111,16 +2111,16 @@
         <v>0.28</v>
       </c>
       <c r="H43" t="n">
-        <v>0.642</v>
+        <v>0.724</v>
       </c>
       <c r="I43" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="K43" t="n">
         <v>0.87</v>
-      </c>
-      <c r="J43" t="n">
-        <v>0.511</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>